<commit_message>
Added logic to persist last saved student between steps
</commit_message>
<xml_diff>
--- a/src/main/resources/students.xlsx
+++ b/src/main/resources/students.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashgarg/personal/learn/gitProjects/SpringBatch 2/src/main/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE4C42C-DB5D-D941-84DE-20BD0D37A26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>NAME</t>
   </si>
@@ -55,13 +61,22 @@
   </si>
   <si>
     <t>PURCHASED_PACKAGE</t>
+  </si>
+  <si>
+    <t>Boris Johnson</t>
+  </si>
+  <si>
+    <t>Michael Jackson</t>
+  </si>
+  <si>
+    <t>Pet Sampras</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -73,6 +88,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,9 +121,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -109,6 +132,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -433,21 +464,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -469,7 +500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -480,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -491,13 +522,50 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" display="mailto:nick.newbie@gmail.com" xr:uid="{877AD197-468A-AF4E-83D5-9614D89308B0}"/>
+    <hyperlink ref="B6" r:id="rId5" display="mailto:nick.newbie@gmail.com" xr:uid="{EA4B8E7B-910E-7B43-8D74-460C95B14448}"/>
+    <hyperlink ref="B7" r:id="rId6" display="mailto:nick.newbie@gmail.com" xr:uid="{9481C8A3-0C04-DF40-87AF-C635EDC1D66B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>